<commit_message>
completing queries in python
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documentos\TEC\BD Avanzadas\P2\bda_neo4j\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0C9148-A341-4C45-B98C-1263157EF0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6950B84-FD0A-443D-BC74-46D2E3F7411A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4198A862-D9AB-4A0C-8678-BEDA35693AEF}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="101">
   <si>
     <t>Consulta 2</t>
   </si>
@@ -301,6 +301,48 @@
   </si>
   <si>
     <t>De todos los que 1(J) sea SI</t>
+  </si>
+  <si>
+    <t>A6: (C) - Servicios</t>
+  </si>
+  <si>
+    <t>A4: (I) - is_Precio_regulado</t>
+  </si>
+  <si>
+    <t>A6: (G) - Piezas_solicitadas</t>
+  </si>
+  <si>
+    <t>A1: (G) - Precio_IVA_euro</t>
+  </si>
+  <si>
+    <t>Separamos por Servicios[6(C)]</t>
+  </si>
+  <si>
+    <t>De cada servicio hacemos top5 de Piezas Solicitadas[6(G)]</t>
+  </si>
+  <si>
+    <t>6(D) con 1(A)</t>
+  </si>
+  <si>
+    <t>6(D) con 4(B)</t>
+  </si>
+  <si>
+    <t>|6(C)|6(D)|1(C)|out de consulta3(6(C))|1(G)|4(I)|</t>
+  </si>
+  <si>
+    <t>A1: (D) - Estado</t>
+  </si>
+  <si>
+    <t>Filtramos los medicamentos por 1(D)=suspendido</t>
+  </si>
+  <si>
+    <t>1(F) con 6(D)</t>
+  </si>
+  <si>
+    <t>Hacemos top10 de princ_act/no sé con respecto a qué, no dice,  pasar machete</t>
+  </si>
+  <si>
+    <t>|#|1(F)|lista 6(D) que tengan 1(F) en 6(D)|</t>
   </si>
 </sst>
 </file>
@@ -316,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,8 +383,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -445,36 +493,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,18 +883,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE51E8F4-48EB-47B2-9926-FA5E2EE83BAE}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -818,334 +912,437 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="16"/>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="16"/>
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="16"/>
       <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="10" t="s">
         <v>18</v>
       </c>
+      <c r="B15" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="9"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C23" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D23" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C24" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14" t="s">
+      <c r="D24" s="9"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="14"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+      <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14" t="s">
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14" t="s">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14" t="s">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="B32" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
+      <c r="B34" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B35" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C35" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D35" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C36" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14" t="s">
+      <c r="D36" s="9"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="14" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14" t="s">
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B40" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C40" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D40" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B42" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C42" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D42" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C43" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="14"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14" t="s">
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A31:A32"/>
+  <mergeCells count="11">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="A23:A31"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A15:A22"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A40:A41"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="A26:A30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1156,13 +1353,13 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
@@ -1181,40 +1378,40 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1224,10 +1421,10 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1237,10 +1434,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1250,31 +1447,31 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1284,34 +1481,34 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>